<commit_message>
IMU to Nav reference
</commit_message>
<xml_diff>
--- a/Hardware/PGN_ACE.xlsx
+++ b/Hardware/PGN_ACE.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="168">
   <si>
     <t>Src</t>
   </si>
@@ -453,9 +453,6 @@
     <t>Subnet Reply to AgIO</t>
   </si>
   <si>
-    <t>From imu/WAS</t>
-  </si>
-  <si>
     <t>ToAutosteer</t>
   </si>
   <si>
@@ -504,24 +501,6 @@
     <t>Rspeed</t>
   </si>
   <si>
-    <t>192.168.5.122</t>
-  </si>
-  <si>
-    <t>Port 5122</t>
-  </si>
-  <si>
-    <t>Steer Module 8888</t>
-  </si>
-  <si>
-    <t>Machine Module 8888</t>
-  </si>
-  <si>
-    <t>GPS 5124</t>
-  </si>
-  <si>
-    <t>GPS/IMU/WAS 5122</t>
-  </si>
-  <si>
     <t>Hello PGN 7777</t>
   </si>
   <si>
@@ -534,7 +513,25 @@
     <t>** 7777 for hello</t>
   </si>
   <si>
-    <t>** 8888 Not used</t>
+    <t>Nav</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Machine Module</t>
+  </si>
+  <si>
+    <t>Steer Module</t>
+  </si>
+  <si>
+    <t>From Nav</t>
+  </si>
+  <si>
+    <t>192.168.5.121</t>
+  </si>
+  <si>
+    <t>Port 5121</t>
   </si>
 </sst>
 </file>
@@ -870,7 +867,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1161,41 +1158,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1504,7 +1500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1518,7 +1514,7 @@
   <dimension ref="B1:AP65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -1657,7 +1653,7 @@
     </row>
     <row r="3" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C3" s="62" t="s">
         <v>72</v>
@@ -1678,17 +1674,17 @@
       <c r="H3" s="19">
         <v>8</v>
       </c>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="104"/>
+      <c r="J3" s="108"/>
       <c r="K3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="105" t="s">
+      <c r="L3" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="106"/>
+      <c r="M3" s="110"/>
       <c r="N3" s="1" t="s">
         <v>114</v>
       </c>
@@ -1742,10 +1738,10 @@
       <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="107" t="s">
+      <c r="N5" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="107"/>
+      <c r="O5" s="111"/>
       <c r="P5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1834,18 +1830,18 @@
       <c r="H9" s="19">
         <v>8</v>
       </c>
-      <c r="I9" s="108" t="s">
+      <c r="I9" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="102"/>
-      <c r="K9" s="107" t="s">
+      <c r="J9" s="113"/>
+      <c r="K9" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="107"/>
-      <c r="M9" s="107" t="s">
+      <c r="L9" s="111"/>
+      <c r="M9" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="107"/>
+      <c r="N9" s="111"/>
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2016,7 +2012,7 @@
     </row>
     <row r="15" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C15" s="57"/>
       <c r="D15" s="66"/>
@@ -2474,7 +2470,7 @@
     </row>
     <row r="26" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D26" s="66" t="s">
         <v>12</v>
@@ -2483,7 +2479,7 @@
         <v>127</v>
       </c>
       <c r="F26" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G26" s="48">
         <v>229</v>
@@ -2492,34 +2488,34 @@
         <v>10</v>
       </c>
       <c r="I26" s="92" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="J26" s="94" t="s">
+      <c r="K26" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="K26" s="94" t="s">
+      <c r="L26" s="94" t="s">
         <v>150</v>
       </c>
-      <c r="L26" s="94" t="s">
+      <c r="M26" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="M26" s="94" t="s">
+      <c r="N26" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="N26" s="94" t="s">
+      <c r="O26" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="O26" s="94" t="s">
+      <c r="P26" s="94" t="s">
         <v>154</v>
       </c>
-      <c r="P26" s="94" t="s">
+      <c r="Q26" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="Q26" s="94" t="s">
+      <c r="R26" s="94" t="s">
         <v>156</v>
-      </c>
-      <c r="R26" s="94" t="s">
-        <v>157</v>
       </c>
       <c r="S26" s="94" t="s">
         <v>20</v>
@@ -2779,11 +2775,11 @@
     </row>
     <row r="36" spans="2:40" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C36" s="59"/>
       <c r="D36" s="68"/>
-      <c r="E36" s="111"/>
+      <c r="E36" s="104"/>
       <c r="F36" s="56"/>
       <c r="G36" s="56"/>
       <c r="H36" s="24"/>
@@ -2820,16 +2816,13 @@
       <c r="AM36" s="24"/>
       <c r="AN36" s="24"/>
     </row>
-    <row r="37" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="C37" s="109"/>
+    <row r="37" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="102"/>
       <c r="D37" s="66"/>
-      <c r="E37" s="112"/>
+      <c r="E37" s="105"/>
       <c r="F37" s="53"/>
       <c r="G37" s="53"/>
-      <c r="H37" s="110"/>
+      <c r="H37" s="103"/>
       <c r="I37" s="99"/>
       <c r="J37" s="99"/>
       <c r="K37" s="99"/>
@@ -2865,14 +2858,14 @@
     </row>
     <row r="38" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="76" t="s">
-        <v>166</v>
-      </c>
-      <c r="C38" s="109"/>
+        <v>158</v>
+      </c>
+      <c r="C38" s="102"/>
       <c r="D38" s="66"/>
-      <c r="E38" s="112"/>
+      <c r="E38" s="105"/>
       <c r="F38" s="53"/>
       <c r="G38" s="53"/>
-      <c r="H38" s="110"/>
+      <c r="H38" s="103"/>
       <c r="I38" s="99"/>
       <c r="J38" s="99"/>
       <c r="K38" s="99"/>
@@ -2908,14 +2901,14 @@
     </row>
     <row r="39" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" s="109"/>
+        <v>159</v>
+      </c>
+      <c r="C39" s="102"/>
       <c r="D39" s="66"/>
-      <c r="E39" s="112"/>
+      <c r="E39" s="105"/>
       <c r="F39" s="53"/>
       <c r="G39" s="53"/>
-      <c r="H39" s="110"/>
+      <c r="H39" s="103"/>
       <c r="I39" s="99"/>
       <c r="J39" s="99"/>
       <c r="K39" s="99"/>
@@ -2950,11 +2943,11 @@
       <c r="AN39" s="99"/>
     </row>
     <row r="40" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="113" t="s">
-        <v>168</v>
+      <c r="B40" s="76" t="s">
+        <v>160</v>
       </c>
       <c r="C40" s="3"/>
-      <c r="E40" s="112"/>
+      <c r="E40" s="105"/>
       <c r="F40" s="53"/>
       <c r="G40" s="53"/>
       <c r="H40" s="101"/>
@@ -2992,7 +2985,7 @@
       <c r="AN40" s="97"/>
     </row>
     <row r="41" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="114"/>
+      <c r="B41" s="106"/>
       <c r="C41" s="3"/>
       <c r="E41" s="52"/>
       <c r="F41" s="53"/>
@@ -3033,10 +3026,10 @@
     </row>
     <row r="42" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="57" t="s">
         <v>141</v>
-      </c>
-      <c r="C42" s="57" t="s">
-        <v>142</v>
       </c>
       <c r="D42" s="66">
         <v>79</v>
@@ -3045,7 +3038,7 @@
         <v>122</v>
       </c>
       <c r="F42" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G42" s="48">
         <v>249</v>
@@ -3054,10 +3047,10 @@
         <v>8</v>
       </c>
       <c r="I42" s="95" t="s">
+        <v>143</v>
+      </c>
+      <c r="J42" s="97" t="s">
         <v>144</v>
-      </c>
-      <c r="J42" s="97" t="s">
-        <v>145</v>
       </c>
       <c r="K42" s="97"/>
       <c r="L42" s="97"/>
@@ -3092,7 +3085,7 @@
     </row>
     <row r="43" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="10" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="H43" s="96"/>
       <c r="I43" s="95"/>
@@ -3130,7 +3123,7 @@
     </row>
     <row r="44" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="10" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="H44" s="96"/>
       <c r="I44" s="95"/>
@@ -3288,7 +3281,7 @@
     </row>
     <row r="48" spans="2:40" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C48" s="59"/>
       <c r="D48" s="68"/>
@@ -4187,9 +4180,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4357,26 +4353,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4400,9 +4385,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>